<commit_message>
Changes in disclosures and burning changes
</commit_message>
<xml_diff>
--- a/phpdocx/template/burning.xlsx
+++ b/phpdocx/template/burning.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>FY 14/15</t>
+  </si>
+  <si>
+    <t>FY14/15</t>
+  </si>
+  <si>
+    <t>FY13/14</t>
+  </si>
+  <si>
+    <t>FY12/13</t>
+  </si>
+  <si>
+    <t>FY11/12</t>
+  </si>
+  <si>
+    <t>FY10/11</t>
+  </si>
+  <si>
+    <t>FY 09/10</t>
   </si>
 </sst>
 </file>
@@ -205,7 +223,7 @@
     <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -263,6 +281,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -613,11 +643,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -726,9 +758,11 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Comma 4" xfId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1022,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F518"/>
+  <dimension ref="B3:F537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C493" sqref="C493:D496"/>
+    <sheetView tabSelected="1" topLeftCell="A511" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J529" sqref="J529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1694,9 +1728,103 @@
       </c>
       <c r="F518" s="50"/>
     </row>
+    <row r="530" spans="2:5" ht="15" thickBot="1"/>
+    <row r="531" spans="2:5">
+      <c r="B531" s="25"/>
+      <c r="C531" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D531" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E531" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="532" spans="2:5">
+      <c r="B532" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C532" s="29">
+        <v>2</v>
+      </c>
+      <c r="D532" s="29">
+        <v>111.3821138211382</v>
+      </c>
+      <c r="E532" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="533" spans="2:5">
+      <c r="B533" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C533" s="29">
+        <v>3</v>
+      </c>
+      <c r="D533" s="29">
+        <v>116.26016260162602</v>
+      </c>
+      <c r="E533" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="534" spans="2:5">
+      <c r="B534" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C534" s="29">
+        <v>4</v>
+      </c>
+      <c r="D534" s="29">
+        <v>122.76422764227641</v>
+      </c>
+      <c r="E534" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="535" spans="2:5">
+      <c r="B535" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C535" s="29">
+        <v>5</v>
+      </c>
+      <c r="D535" s="29">
+        <v>119.51219512195121</v>
+      </c>
+      <c r="E535" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="536" spans="2:5" ht="15" thickBot="1">
+      <c r="B536" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C536" s="32">
+        <v>6</v>
+      </c>
+      <c r="D536" s="32">
+        <v>123.57723577235772</v>
+      </c>
+      <c r="E536" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="537" spans="2:5" ht="15" thickBot="1">
+      <c r="B537" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C537" s="32"/>
+      <c r="D537" s="32"/>
+      <c r="E537" s="33">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
changes in appointment of auditors
</commit_message>
<xml_diff>
--- a/phpdocx/template/burning.xlsx
+++ b/phpdocx/template/burning.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Shareholding Pattern</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>FY 14/15</t>
+  </si>
+  <si>
+    <t>FY14/15</t>
+  </si>
+  <si>
+    <t>FY13/14</t>
+  </si>
+  <si>
+    <t>FY12/13</t>
+  </si>
+  <si>
+    <t>FY11/12</t>
+  </si>
+  <si>
+    <t>FY10/11</t>
+  </si>
+  <si>
+    <t>FY 09/10</t>
   </si>
 </sst>
 </file>
@@ -205,7 +223,7 @@
     <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="167" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -263,6 +281,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="10">
@@ -613,11 +643,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -726,9 +758,11 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Comma 2" xfId="2"/>
     <cellStyle name="Comma 4" xfId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1022,10 +1056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F518"/>
+  <dimension ref="B3:F537"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="C493" sqref="C493:D496"/>
+    <sheetView tabSelected="1" topLeftCell="A511" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J529" sqref="J529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1694,9 +1728,103 @@
       </c>
       <c r="F518" s="50"/>
     </row>
+    <row r="530" spans="2:5" ht="15" thickBot="1"/>
+    <row r="531" spans="2:5">
+      <c r="B531" s="25"/>
+      <c r="C531" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D531" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E531" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="532" spans="2:5">
+      <c r="B532" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C532" s="29">
+        <v>2</v>
+      </c>
+      <c r="D532" s="29">
+        <v>111.3821138211382</v>
+      </c>
+      <c r="E532" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="533" spans="2:5">
+      <c r="B533" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C533" s="29">
+        <v>3</v>
+      </c>
+      <c r="D533" s="29">
+        <v>116.26016260162602</v>
+      </c>
+      <c r="E533" s="30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="534" spans="2:5">
+      <c r="B534" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C534" s="29">
+        <v>4</v>
+      </c>
+      <c r="D534" s="29">
+        <v>122.76422764227641</v>
+      </c>
+      <c r="E534" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="535" spans="2:5">
+      <c r="B535" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C535" s="29">
+        <v>5</v>
+      </c>
+      <c r="D535" s="29">
+        <v>119.51219512195121</v>
+      </c>
+      <c r="E535" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="536" spans="2:5" ht="15" thickBot="1">
+      <c r="B536" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C536" s="32">
+        <v>6</v>
+      </c>
+      <c r="D536" s="32">
+        <v>123.57723577235772</v>
+      </c>
+      <c r="E536" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="537" spans="2:5" ht="15" thickBot="1">
+      <c r="B537" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C537" s="32"/>
+      <c r="D537" s="32"/>
+      <c r="E537" s="33">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>